<commit_message>
Modification du formatage des cellules
</commit_message>
<xml_diff>
--- a/xlsx/modele_indices.xlsx
+++ b/xlsx/modele_indices.xlsx
@@ -125,7 +125,7 @@
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0&quot; €&quot;;[RED]\-#,##0&quot; €&quot;"/>
     <numFmt numFmtId="167" formatCode="General"/>
-    <numFmt numFmtId="168" formatCode="yy/mm/dd"/>
+    <numFmt numFmtId="168" formatCode="[$-409]yyyy/mm/dd"/>
     <numFmt numFmtId="169" formatCode="[$-409]0.00"/>
     <numFmt numFmtId="170" formatCode="0.00\ %"/>
     <numFmt numFmtId="171" formatCode="[$-409]0.00%"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="E2:E550 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2676,11 +2676,11 @@
   <dimension ref="A1:O550"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="13" ySplit="17" topLeftCell="N43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="13" ySplit="17" topLeftCell="N540" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
-      <selection pane="bottomRight" activeCell="P17" activeCellId="0" sqref="P17"/>
+      <selection pane="bottomLeft" activeCell="A540" activeCellId="0" sqref="A540"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2:E550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Update modele_actions.xlsx and modele_indices.xlsx
</commit_message>
<xml_diff>
--- a/xlsx/modele_indices.xlsx
+++ b/xlsx/modele_indices.xlsx
@@ -124,14 +124,14 @@
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0&quot; €&quot;;[RED]\-#,##0&quot; €&quot;"/>
-    <numFmt numFmtId="167" formatCode="[$-409]yyyy/mm/dd"/>
-    <numFmt numFmtId="168" formatCode="[$-409]0.00"/>
-    <numFmt numFmtId="169" formatCode="[$-409]0.00%"/>
-    <numFmt numFmtId="170" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="[$-409]yyyy/mm/dd"/>
+    <numFmt numFmtId="169" formatCode="[$-409]0.00"/>
+    <numFmt numFmtId="170" formatCode="[$-409]0.00%"/>
     <numFmt numFmtId="171" formatCode="[$-409]#,##0"/>
     <numFmt numFmtId="172" formatCode="[$-409]mm/dd/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -179,6 +179,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -344,7 +351,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,11 +369,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -385,16 +388,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="171" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -413,7 +416,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="171" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2701,22 +2712,28 @@
   <dimension ref="A1:P150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="P23" activeCellId="0" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.91"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="25.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2814,14 +2831,14 @@
       </c>
       <c r="M2" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E2,2),"/",MID(EXPORT!E2,4,2),"/",MID(EXPORT!E2,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N2" s="8" t="n">
         <f aca="false">J2/M2*30</f>
-        <v>0.121951219512195</v>
+        <v>0.128205128205128</v>
       </c>
       <c r="O2" s="10" t="n">
-        <f aca="false">MAX(N2-0.005,0)*100*MAX(ABS(L2)-0.2,0)*2*IF(IF(M2&gt;=384,0,M2)&gt;0,(384-M2)/384,0)*10000</f>
+        <f aca="false">MAX(N2-0.005,0)*MAX(ABS(L2)-0.25,0)*IF(IF(M2&gt;=384,0,M2)&gt;0,(384-M2)/384,0)*10000000</f>
         <v>0</v>
       </c>
       <c r="P2" s="11"/>
@@ -2877,14 +2894,14 @@
       </c>
       <c r="M3" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E3,2),"/",MID(EXPORT!E3,4,2),"/",MID(EXPORT!E3,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N3" s="15" t="n">
         <f aca="false">J3/M3*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O3" s="17" t="n">
-        <f aca="false">MAX(N3-0.005,0)*100*MAX(ABS(L3)-0.2,0)*2*IF(IF(M3&gt;=384,0,M3)&gt;0,(384-M3)/384,0)*10000</f>
+        <f aca="false">MAX(N3-0.005,0)*MAX(ABS(L3)-0.25,0)*IF(IF(M3&gt;=384,0,M3)&gt;0,(384-M3)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -2939,14 +2956,14 @@
       </c>
       <c r="M4" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E4,2),"/",MID(EXPORT!E4,4,2),"/",MID(EXPORT!E4,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N4" s="8" t="n">
         <f aca="false">J4/M4*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O4" s="10" t="n">
-        <f aca="false">MAX(N4-0.005,0)*100*MAX(ABS(L4)-0.2,0)*2*IF(IF(M4&gt;=384,0,M4)&gt;0,(384-M4)/384,0)*10000</f>
+        <f aca="false">MAX(N4-0.005,0)*MAX(ABS(L4)-0.25,0)*IF(IF(M4&gt;=384,0,M4)&gt;0,(384-M4)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3001,14 +3018,14 @@
       </c>
       <c r="M5" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E5,2),"/",MID(EXPORT!E5,4,2),"/",MID(EXPORT!E5,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N5" s="15" t="n">
         <f aca="false">J5/M5*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O5" s="17" t="n">
-        <f aca="false">MAX(N5-0.005,0)*100*MAX(ABS(L5)-0.2,0)*2*IF(IF(M5&gt;=384,0,M5)&gt;0,(384-M5)/384,0)*10000</f>
+        <f aca="false">MAX(N5-0.005,0)*MAX(ABS(L5)-0.25,0)*IF(IF(M5&gt;=384,0,M5)&gt;0,(384-M5)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3063,14 +3080,14 @@
       </c>
       <c r="M6" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E6,2),"/",MID(EXPORT!E6,4,2),"/",MID(EXPORT!E6,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N6" s="8" t="n">
         <f aca="false">J6/M6*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O6" s="10" t="n">
-        <f aca="false">MAX(N6-0.005,0)*100*MAX(ABS(L6)-0.2,0)*2*IF(IF(M6&gt;=384,0,M6)&gt;0,(384-M6)/384,0)*10000</f>
+        <f aca="false">MAX(N6-0.005,0)*MAX(ABS(L6)-0.25,0)*IF(IF(M6&gt;=384,0,M6)&gt;0,(384-M6)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3125,14 +3142,14 @@
       </c>
       <c r="M7" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E7,2),"/",MID(EXPORT!E7,4,2),"/",MID(EXPORT!E7,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N7" s="15" t="n">
         <f aca="false">J7/M7*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O7" s="17" t="n">
-        <f aca="false">MAX(N7-0.005,0)*100*MAX(ABS(L7)-0.2,0)*2*IF(IF(M7&gt;=384,0,M7)&gt;0,(384-M7)/384,0)*10000</f>
+        <f aca="false">MAX(N7-0.005,0)*MAX(ABS(L7)-0.25,0)*IF(IF(M7&gt;=384,0,M7)&gt;0,(384-M7)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3187,14 +3204,14 @@
       </c>
       <c r="M8" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E8,2),"/",MID(EXPORT!E8,4,2),"/",MID(EXPORT!E8,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N8" s="8" t="n">
         <f aca="false">J8/M8*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O8" s="10" t="n">
-        <f aca="false">MAX(N8-0.005,0)*100*MAX(ABS(L8)-0.2,0)*2*IF(IF(M8&gt;=384,0,M8)&gt;0,(384-M8)/384,0)*10000</f>
+        <f aca="false">MAX(N8-0.005,0)*MAX(ABS(L8)-0.25,0)*IF(IF(M8&gt;=384,0,M8)&gt;0,(384-M8)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3249,14 +3266,14 @@
       </c>
       <c r="M9" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E9,2),"/",MID(EXPORT!E9,4,2),"/",MID(EXPORT!E9,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N9" s="15" t="n">
         <f aca="false">J9/M9*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O9" s="17" t="n">
-        <f aca="false">MAX(N9-0.005,0)*100*MAX(ABS(L9)-0.2,0)*2*IF(IF(M9&gt;=384,0,M9)&gt;0,(384-M9)/384,0)*10000</f>
+        <f aca="false">MAX(N9-0.005,0)*MAX(ABS(L9)-0.25,0)*IF(IF(M9&gt;=384,0,M9)&gt;0,(384-M9)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3311,14 +3328,14 @@
       </c>
       <c r="M10" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E10,2),"/",MID(EXPORT!E10,4,2),"/",MID(EXPORT!E10,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N10" s="8" t="n">
         <f aca="false">J10/M10*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O10" s="10" t="n">
-        <f aca="false">MAX(N10-0.005,0)*100*MAX(ABS(L10)-0.2,0)*2*IF(IF(M10&gt;=384,0,M10)&gt;0,(384-M10)/384,0)*10000</f>
+        <f aca="false">MAX(N10-0.005,0)*MAX(ABS(L10)-0.25,0)*IF(IF(M10&gt;=384,0,M10)&gt;0,(384-M10)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3373,14 +3390,14 @@
       </c>
       <c r="M11" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E11,2),"/",MID(EXPORT!E11,4,2),"/",MID(EXPORT!E11,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N11" s="15" t="n">
         <f aca="false">J11/M11*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O11" s="17" t="n">
-        <f aca="false">MAX(N11-0.005,0)*100*MAX(ABS(L11)-0.2,0)*2*IF(IF(M11&gt;=384,0,M11)&gt;0,(384-M11)/384,0)*10000</f>
+        <f aca="false">MAX(N11-0.005,0)*MAX(ABS(L11)-0.25,0)*IF(IF(M11&gt;=384,0,M11)&gt;0,(384-M11)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3435,14 +3452,14 @@
       </c>
       <c r="M12" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E12,2),"/",MID(EXPORT!E12,4,2),"/",MID(EXPORT!E12,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N12" s="8" t="n">
         <f aca="false">J12/M12*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O12" s="10" t="n">
-        <f aca="false">MAX(N12-0.005,0)*100*MAX(ABS(L12)-0.2,0)*2*IF(IF(M12&gt;=384,0,M12)&gt;0,(384-M12)/384,0)*10000</f>
+        <f aca="false">MAX(N12-0.005,0)*MAX(ABS(L12)-0.25,0)*IF(IF(M12&gt;=384,0,M12)&gt;0,(384-M12)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3497,14 +3514,14 @@
       </c>
       <c r="M13" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E13,2),"/",MID(EXPORT!E13,4,2),"/",MID(EXPORT!E13,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N13" s="15" t="n">
         <f aca="false">J13/M13*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O13" s="17" t="n">
-        <f aca="false">MAX(N13-0.005,0)*100*MAX(ABS(L13)-0.2,0)*2*IF(IF(M13&gt;=384,0,M13)&gt;0,(384-M13)/384,0)*10000</f>
+        <f aca="false">MAX(N13-0.005,0)*MAX(ABS(L13)-0.25,0)*IF(IF(M13&gt;=384,0,M13)&gt;0,(384-M13)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3559,14 +3576,14 @@
       </c>
       <c r="M14" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E14,2),"/",MID(EXPORT!E14,4,2),"/",MID(EXPORT!E14,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N14" s="8" t="n">
         <f aca="false">J14/M14*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O14" s="10" t="n">
-        <f aca="false">MAX(N14-0.005,0)*100*MAX(ABS(L14)-0.2,0)*2*IF(IF(M14&gt;=384,0,M14)&gt;0,(384-M14)/384,0)*10000</f>
+        <f aca="false">MAX(N14-0.005,0)*MAX(ABS(L14)-0.25,0)*IF(IF(M14&gt;=384,0,M14)&gt;0,(384-M14)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3621,14 +3638,14 @@
       </c>
       <c r="M15" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E15,2),"/",MID(EXPORT!E15,4,2),"/",MID(EXPORT!E15,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N15" s="15" t="n">
         <f aca="false">J15/M15*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O15" s="17" t="n">
-        <f aca="false">MAX(N15-0.005,0)*100*MAX(ABS(L15)-0.2,0)*2*IF(IF(M15&gt;=384,0,M15)&gt;0,(384-M15)/384,0)*10000</f>
+        <f aca="false">MAX(N15-0.005,0)*MAX(ABS(L15)-0.25,0)*IF(IF(M15&gt;=384,0,M15)&gt;0,(384-M15)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3683,14 +3700,14 @@
       </c>
       <c r="M16" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E16,2),"/",MID(EXPORT!E16,4,2),"/",MID(EXPORT!E16,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N16" s="8" t="n">
         <f aca="false">J16/M16*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O16" s="10" t="n">
-        <f aca="false">MAX(N16-0.005,0)*100*MAX(ABS(L16)-0.2,0)*2*IF(IF(M16&gt;=384,0,M16)&gt;0,(384-M16)/384,0)*10000</f>
+        <f aca="false">MAX(N16-0.005,0)*MAX(ABS(L16)-0.25,0)*IF(IF(M16&gt;=384,0,M16)&gt;0,(384-M16)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3745,14 +3762,14 @@
       </c>
       <c r="M17" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E17,2),"/",MID(EXPORT!E17,4,2),"/",MID(EXPORT!E17,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N17" s="15" t="n">
         <f aca="false">J17/M17*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O17" s="17" t="n">
-        <f aca="false">MAX(N17-0.005,0)*100*MAX(ABS(L17)-0.2,0)*2*IF(IF(M17&gt;=384,0,M17)&gt;0,(384-M17)/384,0)*10000</f>
+        <f aca="false">MAX(N17-0.005,0)*MAX(ABS(L17)-0.25,0)*IF(IF(M17&gt;=384,0,M17)&gt;0,(384-M17)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3807,14 +3824,14 @@
       </c>
       <c r="M18" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E18,2),"/",MID(EXPORT!E18,4,2),"/",MID(EXPORT!E18,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N18" s="8" t="n">
         <f aca="false">J18/M18*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O18" s="10" t="n">
-        <f aca="false">MAX(N18-0.005,0)*100*MAX(ABS(L18)-0.2,0)*2*IF(IF(M18&gt;=384,0,M18)&gt;0,(384-M18)/384,0)*10000</f>
+        <f aca="false">MAX(N18-0.005,0)*MAX(ABS(L18)-0.25,0)*IF(IF(M18&gt;=384,0,M18)&gt;0,(384-M18)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3869,14 +3886,14 @@
       </c>
       <c r="M19" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E19,2),"/",MID(EXPORT!E19,4,2),"/",MID(EXPORT!E19,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N19" s="15" t="n">
         <f aca="false">J19/M19*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O19" s="17" t="n">
-        <f aca="false">MAX(N19-0.005,0)*100*MAX(ABS(L19)-0.2,0)*2*IF(IF(M19&gt;=384,0,M19)&gt;0,(384-M19)/384,0)*10000</f>
+        <f aca="false">MAX(N19-0.005,0)*MAX(ABS(L19)-0.25,0)*IF(IF(M19&gt;=384,0,M19)&gt;0,(384-M19)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3931,14 +3948,14 @@
       </c>
       <c r="M20" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E20,2),"/",MID(EXPORT!E20,4,2),"/",MID(EXPORT!E20,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N20" s="8" t="n">
         <f aca="false">J20/M20*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O20" s="10" t="n">
-        <f aca="false">MAX(N20-0.005,0)*100*MAX(ABS(L20)-0.2,0)*2*IF(IF(M20&gt;=384,0,M20)&gt;0,(384-M20)/384,0)*10000</f>
+        <f aca="false">MAX(N20-0.005,0)*MAX(ABS(L20)-0.25,0)*IF(IF(M20&gt;=384,0,M20)&gt;0,(384-M20)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -3993,14 +4010,14 @@
       </c>
       <c r="M21" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E21,2),"/",MID(EXPORT!E21,4,2),"/",MID(EXPORT!E21,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N21" s="15" t="n">
         <f aca="false">J21/M21*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O21" s="17" t="n">
-        <f aca="false">MAX(N21-0.005,0)*100*MAX(ABS(L21)-0.2,0)*2*IF(IF(M21&gt;=384,0,M21)&gt;0,(384-M21)/384,0)*10000</f>
+        <f aca="false">MAX(N21-0.005,0)*MAX(ABS(L21)-0.25,0)*IF(IF(M21&gt;=384,0,M21)&gt;0,(384-M21)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4055,14 +4072,14 @@
       </c>
       <c r="M22" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E22,2),"/",MID(EXPORT!E22,4,2),"/",MID(EXPORT!E22,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N22" s="8" t="n">
         <f aca="false">J22/M22*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O22" s="10" t="n">
-        <f aca="false">MAX(N22-0.005,0)*100*MAX(ABS(L22)-0.2,0)*2*IF(IF(M22&gt;=384,0,M22)&gt;0,(384-M22)/384,0)*10000</f>
+        <f aca="false">MAX(N22-0.005,0)*MAX(ABS(L22)-0.25,0)*IF(IF(M22&gt;=384,0,M22)&gt;0,(384-M22)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4117,14 +4134,14 @@
       </c>
       <c r="M23" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E23,2),"/",MID(EXPORT!E23,4,2),"/",MID(EXPORT!E23,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N23" s="15" t="n">
         <f aca="false">J23/M23*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O23" s="17" t="n">
-        <f aca="false">MAX(N23-0.005,0)*100*MAX(ABS(L23)-0.2,0)*2*IF(IF(M23&gt;=384,0,M23)&gt;0,(384-M23)/384,0)*10000</f>
+        <f aca="false">MAX(N23-0.005,0)*MAX(ABS(L23)-0.25,0)*IF(IF(M23&gt;=384,0,M23)&gt;0,(384-M23)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4179,14 +4196,14 @@
       </c>
       <c r="M24" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E24,2),"/",MID(EXPORT!E24,4,2),"/",MID(EXPORT!E24,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N24" s="8" t="n">
         <f aca="false">J24/M24*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O24" s="10" t="n">
-        <f aca="false">MAX(N24-0.005,0)*100*MAX(ABS(L24)-0.2,0)*2*IF(IF(M24&gt;=384,0,M24)&gt;0,(384-M24)/384,0)*10000</f>
+        <f aca="false">MAX(N24-0.005,0)*MAX(ABS(L24)-0.25,0)*IF(IF(M24&gt;=384,0,M24)&gt;0,(384-M24)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4241,14 +4258,14 @@
       </c>
       <c r="M25" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E25,2),"/",MID(EXPORT!E25,4,2),"/",MID(EXPORT!E25,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N25" s="15" t="n">
         <f aca="false">J25/M25*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O25" s="17" t="n">
-        <f aca="false">MAX(N25-0.005,0)*100*MAX(ABS(L25)-0.2,0)*2*IF(IF(M25&gt;=384,0,M25)&gt;0,(384-M25)/384,0)*10000</f>
+        <f aca="false">MAX(N25-0.005,0)*MAX(ABS(L25)-0.25,0)*IF(IF(M25&gt;=384,0,M25)&gt;0,(384-M25)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4303,14 +4320,14 @@
       </c>
       <c r="M26" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E26,2),"/",MID(EXPORT!E26,4,2),"/",MID(EXPORT!E26,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N26" s="8" t="n">
         <f aca="false">J26/M26*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O26" s="10" t="n">
-        <f aca="false">MAX(N26-0.005,0)*100*MAX(ABS(L26)-0.2,0)*2*IF(IF(M26&gt;=384,0,M26)&gt;0,(384-M26)/384,0)*10000</f>
+        <f aca="false">MAX(N26-0.005,0)*MAX(ABS(L26)-0.25,0)*IF(IF(M26&gt;=384,0,M26)&gt;0,(384-M26)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4365,14 +4382,14 @@
       </c>
       <c r="M27" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E27,2),"/",MID(EXPORT!E27,4,2),"/",MID(EXPORT!E27,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N27" s="15" t="n">
         <f aca="false">J27/M27*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O27" s="17" t="n">
-        <f aca="false">MAX(N27-0.005,0)*100*MAX(ABS(L27)-0.2,0)*2*IF(IF(M27&gt;=384,0,M27)&gt;0,(384-M27)/384,0)*10000</f>
+        <f aca="false">MAX(N27-0.005,0)*MAX(ABS(L27)-0.25,0)*IF(IF(M27&gt;=384,0,M27)&gt;0,(384-M27)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4427,14 +4444,14 @@
       </c>
       <c r="M28" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E28,2),"/",MID(EXPORT!E28,4,2),"/",MID(EXPORT!E28,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N28" s="8" t="n">
         <f aca="false">J28/M28*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O28" s="10" t="n">
-        <f aca="false">MAX(N28-0.005,0)*100*MAX(ABS(L28)-0.2,0)*2*IF(IF(M28&gt;=384,0,M28)&gt;0,(384-M28)/384,0)*10000</f>
+        <f aca="false">MAX(N28-0.005,0)*MAX(ABS(L28)-0.25,0)*IF(IF(M28&gt;=384,0,M28)&gt;0,(384-M28)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4489,14 +4506,14 @@
       </c>
       <c r="M29" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E29,2),"/",MID(EXPORT!E29,4,2),"/",MID(EXPORT!E29,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N29" s="15" t="n">
         <f aca="false">J29/M29*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O29" s="17" t="n">
-        <f aca="false">MAX(N29-0.005,0)*100*MAX(ABS(L29)-0.2,0)*2*IF(IF(M29&gt;=384,0,M29)&gt;0,(384-M29)/384,0)*10000</f>
+        <f aca="false">MAX(N29-0.005,0)*MAX(ABS(L29)-0.25,0)*IF(IF(M29&gt;=384,0,M29)&gt;0,(384-M29)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4551,14 +4568,14 @@
       </c>
       <c r="M30" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E30,2),"/",MID(EXPORT!E30,4,2),"/",MID(EXPORT!E30,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N30" s="8" t="n">
         <f aca="false">J30/M30*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O30" s="10" t="n">
-        <f aca="false">MAX(N30-0.005,0)*100*MAX(ABS(L30)-0.2,0)*2*IF(IF(M30&gt;=384,0,M30)&gt;0,(384-M30)/384,0)*10000</f>
+        <f aca="false">MAX(N30-0.005,0)*MAX(ABS(L30)-0.25,0)*IF(IF(M30&gt;=384,0,M30)&gt;0,(384-M30)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4613,14 +4630,14 @@
       </c>
       <c r="M31" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E31,2),"/",MID(EXPORT!E31,4,2),"/",MID(EXPORT!E31,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N31" s="15" t="n">
         <f aca="false">J31/M31*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O31" s="17" t="n">
-        <f aca="false">MAX(N31-0.005,0)*100*MAX(ABS(L31)-0.2,0)*2*IF(IF(M31&gt;=384,0,M31)&gt;0,(384-M31)/384,0)*10000</f>
+        <f aca="false">MAX(N31-0.005,0)*MAX(ABS(L31)-0.25,0)*IF(IF(M31&gt;=384,0,M31)&gt;0,(384-M31)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4675,14 +4692,14 @@
       </c>
       <c r="M32" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E32,2),"/",MID(EXPORT!E32,4,2),"/",MID(EXPORT!E32,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N32" s="8" t="n">
         <f aca="false">J32/M32*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O32" s="10" t="n">
-        <f aca="false">MAX(N32-0.005,0)*100*MAX(ABS(L32)-0.2,0)*2*IF(IF(M32&gt;=384,0,M32)&gt;0,(384-M32)/384,0)*10000</f>
+        <f aca="false">MAX(N32-0.005,0)*MAX(ABS(L32)-0.25,0)*IF(IF(M32&gt;=384,0,M32)&gt;0,(384-M32)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4737,14 +4754,14 @@
       </c>
       <c r="M33" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E33,2),"/",MID(EXPORT!E33,4,2),"/",MID(EXPORT!E33,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N33" s="15" t="n">
         <f aca="false">J33/M33*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O33" s="17" t="n">
-        <f aca="false">MAX(N33-0.005,0)*100*MAX(ABS(L33)-0.2,0)*2*IF(IF(M33&gt;=384,0,M33)&gt;0,(384-M33)/384,0)*10000</f>
+        <f aca="false">MAX(N33-0.005,0)*MAX(ABS(L33)-0.25,0)*IF(IF(M33&gt;=384,0,M33)&gt;0,(384-M33)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4799,14 +4816,14 @@
       </c>
       <c r="M34" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E34,2),"/",MID(EXPORT!E34,4,2),"/",MID(EXPORT!E34,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N34" s="8" t="n">
         <f aca="false">J34/M34*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O34" s="10" t="n">
-        <f aca="false">MAX(N34-0.005,0)*100*MAX(ABS(L34)-0.2,0)*2*IF(IF(M34&gt;=384,0,M34)&gt;0,(384-M34)/384,0)*10000</f>
+        <f aca="false">MAX(N34-0.005,0)*MAX(ABS(L34)-0.25,0)*IF(IF(M34&gt;=384,0,M34)&gt;0,(384-M34)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4861,14 +4878,14 @@
       </c>
       <c r="M35" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E35,2),"/",MID(EXPORT!E35,4,2),"/",MID(EXPORT!E35,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N35" s="15" t="n">
         <f aca="false">J35/M35*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O35" s="17" t="n">
-        <f aca="false">MAX(N35-0.005,0)*100*MAX(ABS(L35)-0.2,0)*2*IF(IF(M35&gt;=384,0,M35)&gt;0,(384-M35)/384,0)*10000</f>
+        <f aca="false">MAX(N35-0.005,0)*MAX(ABS(L35)-0.25,0)*IF(IF(M35&gt;=384,0,M35)&gt;0,(384-M35)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4923,14 +4940,14 @@
       </c>
       <c r="M36" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E36,2),"/",MID(EXPORT!E36,4,2),"/",MID(EXPORT!E36,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N36" s="8" t="n">
         <f aca="false">J36/M36*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O36" s="10" t="n">
-        <f aca="false">MAX(N36-0.005,0)*100*MAX(ABS(L36)-0.2,0)*2*IF(IF(M36&gt;=384,0,M36)&gt;0,(384-M36)/384,0)*10000</f>
+        <f aca="false">MAX(N36-0.005,0)*MAX(ABS(L36)-0.25,0)*IF(IF(M36&gt;=384,0,M36)&gt;0,(384-M36)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -4985,14 +5002,14 @@
       </c>
       <c r="M37" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E37,2),"/",MID(EXPORT!E37,4,2),"/",MID(EXPORT!E37,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N37" s="15" t="n">
         <f aca="false">J37/M37*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O37" s="17" t="n">
-        <f aca="false">MAX(N37-0.005,0)*100*MAX(ABS(L37)-0.2,0)*2*IF(IF(M37&gt;=384,0,M37)&gt;0,(384-M37)/384,0)*10000</f>
+        <f aca="false">MAX(N37-0.005,0)*MAX(ABS(L37)-0.25,0)*IF(IF(M37&gt;=384,0,M37)&gt;0,(384-M37)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5047,14 +5064,14 @@
       </c>
       <c r="M38" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E38,2),"/",MID(EXPORT!E38,4,2),"/",MID(EXPORT!E38,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N38" s="8" t="n">
         <f aca="false">J38/M38*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O38" s="10" t="n">
-        <f aca="false">MAX(N38-0.005,0)*100*MAX(ABS(L38)-0.2,0)*2*IF(IF(M38&gt;=384,0,M38)&gt;0,(384-M38)/384,0)*10000</f>
+        <f aca="false">MAX(N38-0.005,0)*MAX(ABS(L38)-0.25,0)*IF(IF(M38&gt;=384,0,M38)&gt;0,(384-M38)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5109,14 +5126,14 @@
       </c>
       <c r="M39" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E39,2),"/",MID(EXPORT!E39,4,2),"/",MID(EXPORT!E39,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N39" s="15" t="n">
         <f aca="false">J39/M39*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O39" s="17" t="n">
-        <f aca="false">MAX(N39-0.005,0)*100*MAX(ABS(L39)-0.2,0)*2*IF(IF(M39&gt;=384,0,M39)&gt;0,(384-M39)/384,0)*10000</f>
+        <f aca="false">MAX(N39-0.005,0)*MAX(ABS(L39)-0.25,0)*IF(IF(M39&gt;=384,0,M39)&gt;0,(384-M39)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5171,14 +5188,14 @@
       </c>
       <c r="M40" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E40,2),"/",MID(EXPORT!E40,4,2),"/",MID(EXPORT!E40,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N40" s="8" t="n">
         <f aca="false">J40/M40*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O40" s="10" t="n">
-        <f aca="false">MAX(N40-0.005,0)*100*MAX(ABS(L40)-0.2,0)*2*IF(IF(M40&gt;=384,0,M40)&gt;0,(384-M40)/384,0)*10000</f>
+        <f aca="false">MAX(N40-0.005,0)*MAX(ABS(L40)-0.25,0)*IF(IF(M40&gt;=384,0,M40)&gt;0,(384-M40)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5233,14 +5250,14 @@
       </c>
       <c r="M41" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E41,2),"/",MID(EXPORT!E41,4,2),"/",MID(EXPORT!E41,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N41" s="15" t="n">
         <f aca="false">J41/M41*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O41" s="17" t="n">
-        <f aca="false">MAX(N41-0.005,0)*100*MAX(ABS(L41)-0.2,0)*2*IF(IF(M41&gt;=384,0,M41)&gt;0,(384-M41)/384,0)*10000</f>
+        <f aca="false">MAX(N41-0.005,0)*MAX(ABS(L41)-0.25,0)*IF(IF(M41&gt;=384,0,M41)&gt;0,(384-M41)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5295,14 +5312,14 @@
       </c>
       <c r="M42" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E42,2),"/",MID(EXPORT!E42,4,2),"/",MID(EXPORT!E42,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N42" s="8" t="n">
         <f aca="false">J42/M42*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O42" s="10" t="n">
-        <f aca="false">MAX(N42-0.005,0)*100*MAX(ABS(L42)-0.2,0)*2*IF(IF(M42&gt;=384,0,M42)&gt;0,(384-M42)/384,0)*10000</f>
+        <f aca="false">MAX(N42-0.005,0)*MAX(ABS(L42)-0.25,0)*IF(IF(M42&gt;=384,0,M42)&gt;0,(384-M42)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5357,14 +5374,14 @@
       </c>
       <c r="M43" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E43,2),"/",MID(EXPORT!E43,4,2),"/",MID(EXPORT!E43,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N43" s="15" t="n">
         <f aca="false">J43/M43*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O43" s="17" t="n">
-        <f aca="false">MAX(N43-0.005,0)*100*MAX(ABS(L43)-0.2,0)*2*IF(IF(M43&gt;=384,0,M43)&gt;0,(384-M43)/384,0)*10000</f>
+        <f aca="false">MAX(N43-0.005,0)*MAX(ABS(L43)-0.25,0)*IF(IF(M43&gt;=384,0,M43)&gt;0,(384-M43)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5419,14 +5436,14 @@
       </c>
       <c r="M44" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E44,2),"/",MID(EXPORT!E44,4,2),"/",MID(EXPORT!E44,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N44" s="8" t="n">
         <f aca="false">J44/M44*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O44" s="10" t="n">
-        <f aca="false">MAX(N44-0.005,0)*100*MAX(ABS(L44)-0.2,0)*2*IF(IF(M44&gt;=384,0,M44)&gt;0,(384-M44)/384,0)*10000</f>
+        <f aca="false">MAX(N44-0.005,0)*MAX(ABS(L44)-0.25,0)*IF(IF(M44&gt;=384,0,M44)&gt;0,(384-M44)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5481,14 +5498,14 @@
       </c>
       <c r="M45" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E45,2),"/",MID(EXPORT!E45,4,2),"/",MID(EXPORT!E45,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N45" s="15" t="n">
         <f aca="false">J45/M45*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O45" s="17" t="n">
-        <f aca="false">MAX(N45-0.005,0)*100*MAX(ABS(L45)-0.2,0)*2*IF(IF(M45&gt;=384,0,M45)&gt;0,(384-M45)/384,0)*10000</f>
+        <f aca="false">MAX(N45-0.005,0)*MAX(ABS(L45)-0.25,0)*IF(IF(M45&gt;=384,0,M45)&gt;0,(384-M45)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5543,14 +5560,14 @@
       </c>
       <c r="M46" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E46,2),"/",MID(EXPORT!E46,4,2),"/",MID(EXPORT!E46,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N46" s="8" t="n">
         <f aca="false">J46/M46*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O46" s="10" t="n">
-        <f aca="false">MAX(N46-0.005,0)*100*MAX(ABS(L46)-0.2,0)*2*IF(IF(M46&gt;=384,0,M46)&gt;0,(384-M46)/384,0)*10000</f>
+        <f aca="false">MAX(N46-0.005,0)*MAX(ABS(L46)-0.25,0)*IF(IF(M46&gt;=384,0,M46)&gt;0,(384-M46)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5605,14 +5622,14 @@
       </c>
       <c r="M47" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E47,2),"/",MID(EXPORT!E47,4,2),"/",MID(EXPORT!E47,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N47" s="15" t="n">
         <f aca="false">J47/M47*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O47" s="17" t="n">
-        <f aca="false">MAX(N47-0.005,0)*100*MAX(ABS(L47)-0.2,0)*2*IF(IF(M47&gt;=384,0,M47)&gt;0,(384-M47)/384,0)*10000</f>
+        <f aca="false">MAX(N47-0.005,0)*MAX(ABS(L47)-0.25,0)*IF(IF(M47&gt;=384,0,M47)&gt;0,(384-M47)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5667,14 +5684,14 @@
       </c>
       <c r="M48" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E48,2),"/",MID(EXPORT!E48,4,2),"/",MID(EXPORT!E48,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N48" s="8" t="n">
         <f aca="false">J48/M48*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O48" s="10" t="n">
-        <f aca="false">MAX(N48-0.005,0)*100*MAX(ABS(L48)-0.2,0)*2*IF(IF(M48&gt;=384,0,M48)&gt;0,(384-M48)/384,0)*10000</f>
+        <f aca="false">MAX(N48-0.005,0)*MAX(ABS(L48)-0.25,0)*IF(IF(M48&gt;=384,0,M48)&gt;0,(384-M48)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5729,14 +5746,14 @@
       </c>
       <c r="M49" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E49,2),"/",MID(EXPORT!E49,4,2),"/",MID(EXPORT!E49,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N49" s="15" t="n">
         <f aca="false">J49/M49*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O49" s="17" t="n">
-        <f aca="false">MAX(N49-0.005,0)*100*MAX(ABS(L49)-0.2,0)*2*IF(IF(M49&gt;=384,0,M49)&gt;0,(384-M49)/384,0)*10000</f>
+        <f aca="false">MAX(N49-0.005,0)*MAX(ABS(L49)-0.25,0)*IF(IF(M49&gt;=384,0,M49)&gt;0,(384-M49)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5791,14 +5808,14 @@
       </c>
       <c r="M50" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E50,2),"/",MID(EXPORT!E50,4,2),"/",MID(EXPORT!E50,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N50" s="8" t="n">
         <f aca="false">J50/M50*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O50" s="10" t="n">
-        <f aca="false">MAX(N50-0.005,0)*100*MAX(ABS(L50)-0.2,0)*2*IF(IF(M50&gt;=384,0,M50)&gt;0,(384-M50)/384,0)*10000</f>
+        <f aca="false">MAX(N50-0.005,0)*MAX(ABS(L50)-0.25,0)*IF(IF(M50&gt;=384,0,M50)&gt;0,(384-M50)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5853,14 +5870,14 @@
       </c>
       <c r="M51" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E51,2),"/",MID(EXPORT!E51,4,2),"/",MID(EXPORT!E51,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N51" s="15" t="n">
         <f aca="false">J51/M51*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O51" s="17" t="n">
-        <f aca="false">MAX(N51-0.005,0)*100*MAX(ABS(L51)-0.2,0)*2*IF(IF(M51&gt;=384,0,M51)&gt;0,(384-M51)/384,0)*10000</f>
+        <f aca="false">MAX(N51-0.005,0)*MAX(ABS(L51)-0.25,0)*IF(IF(M51&gt;=384,0,M51)&gt;0,(384-M51)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5915,14 +5932,14 @@
       </c>
       <c r="M52" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E52,2),"/",MID(EXPORT!E52,4,2),"/",MID(EXPORT!E52,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N52" s="8" t="n">
         <f aca="false">J52/M52*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O52" s="10" t="n">
-        <f aca="false">MAX(N52-0.005,0)*100*MAX(ABS(L52)-0.2,0)*2*IF(IF(M52&gt;=384,0,M52)&gt;0,(384-M52)/384,0)*10000</f>
+        <f aca="false">MAX(N52-0.005,0)*MAX(ABS(L52)-0.25,0)*IF(IF(M52&gt;=384,0,M52)&gt;0,(384-M52)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -5977,14 +5994,14 @@
       </c>
       <c r="M53" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E53,2),"/",MID(EXPORT!E53,4,2),"/",MID(EXPORT!E53,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N53" s="15" t="n">
         <f aca="false">J53/M53*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O53" s="17" t="n">
-        <f aca="false">MAX(N53-0.005,0)*100*MAX(ABS(L53)-0.2,0)*2*IF(IF(M53&gt;=384,0,M53)&gt;0,(384-M53)/384,0)*10000</f>
+        <f aca="false">MAX(N53-0.005,0)*MAX(ABS(L53)-0.25,0)*IF(IF(M53&gt;=384,0,M53)&gt;0,(384-M53)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6039,14 +6056,14 @@
       </c>
       <c r="M54" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E54,2),"/",MID(EXPORT!E54,4,2),"/",MID(EXPORT!E54,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N54" s="8" t="n">
         <f aca="false">J54/M54*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O54" s="10" t="n">
-        <f aca="false">MAX(N54-0.005,0)*100*MAX(ABS(L54)-0.2,0)*2*IF(IF(M54&gt;=384,0,M54)&gt;0,(384-M54)/384,0)*10000</f>
+        <f aca="false">MAX(N54-0.005,0)*MAX(ABS(L54)-0.25,0)*IF(IF(M54&gt;=384,0,M54)&gt;0,(384-M54)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6101,14 +6118,14 @@
       </c>
       <c r="M55" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E55,2),"/",MID(EXPORT!E55,4,2),"/",MID(EXPORT!E55,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N55" s="15" t="n">
         <f aca="false">J55/M55*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O55" s="17" t="n">
-        <f aca="false">MAX(N55-0.005,0)*100*MAX(ABS(L55)-0.2,0)*2*IF(IF(M55&gt;=384,0,M55)&gt;0,(384-M55)/384,0)*10000</f>
+        <f aca="false">MAX(N55-0.005,0)*MAX(ABS(L55)-0.25,0)*IF(IF(M55&gt;=384,0,M55)&gt;0,(384-M55)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6163,14 +6180,14 @@
       </c>
       <c r="M56" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E56,2),"/",MID(EXPORT!E56,4,2),"/",MID(EXPORT!E56,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N56" s="8" t="n">
         <f aca="false">J56/M56*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O56" s="10" t="n">
-        <f aca="false">MAX(N56-0.005,0)*100*MAX(ABS(L56)-0.2,0)*2*IF(IF(M56&gt;=384,0,M56)&gt;0,(384-M56)/384,0)*10000</f>
+        <f aca="false">MAX(N56-0.005,0)*MAX(ABS(L56)-0.25,0)*IF(IF(M56&gt;=384,0,M56)&gt;0,(384-M56)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6225,14 +6242,14 @@
       </c>
       <c r="M57" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E57,2),"/",MID(EXPORT!E57,4,2),"/",MID(EXPORT!E57,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N57" s="15" t="n">
         <f aca="false">J57/M57*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O57" s="17" t="n">
-        <f aca="false">MAX(N57-0.005,0)*100*MAX(ABS(L57)-0.2,0)*2*IF(IF(M57&gt;=384,0,M57)&gt;0,(384-M57)/384,0)*10000</f>
+        <f aca="false">MAX(N57-0.005,0)*MAX(ABS(L57)-0.25,0)*IF(IF(M57&gt;=384,0,M57)&gt;0,(384-M57)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6287,14 +6304,14 @@
       </c>
       <c r="M58" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E58,2),"/",MID(EXPORT!E58,4,2),"/",MID(EXPORT!E58,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N58" s="8" t="n">
         <f aca="false">J58/M58*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O58" s="10" t="n">
-        <f aca="false">MAX(N58-0.005,0)*100*MAX(ABS(L58)-0.2,0)*2*IF(IF(M58&gt;=384,0,M58)&gt;0,(384-M58)/384,0)*10000</f>
+        <f aca="false">MAX(N58-0.005,0)*MAX(ABS(L58)-0.25,0)*IF(IF(M58&gt;=384,0,M58)&gt;0,(384-M58)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6349,14 +6366,14 @@
       </c>
       <c r="M59" s="16" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E59,2),"/",MID(EXPORT!E59,4,2),"/",MID(EXPORT!E59,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N59" s="15" t="n">
         <f aca="false">J59/M59*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O59" s="17" t="n">
-        <f aca="false">MAX(N59-0.005,0)*100*MAX(ABS(L59)-0.2,0)*2*IF(IF(M59&gt;=384,0,M59)&gt;0,(384-M59)/384,0)*10000</f>
+        <f aca="false">MAX(N59-0.005,0)*MAX(ABS(L59)-0.25,0)*IF(IF(M59&gt;=384,0,M59)&gt;0,(384-M59)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6411,14 +6428,14 @@
       </c>
       <c r="M60" s="9" t="n">
         <f aca="true">IFERROR(_xlfn.DAYS(CONCATENATE(LEFT(EXPORT!E60,2),"/",MID(EXPORT!E60,4,2),"/",MID(EXPORT!E60,9,2)),TODAY()),0)</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N60" s="8" t="n">
         <f aca="false">J60/M60*30</f>
-        <v>0.104529616724739</v>
+        <v>0.10989010989011</v>
       </c>
       <c r="O60" s="10" t="n">
-        <f aca="false">MAX(N60-0.005,0)*100*MAX(ABS(L60)-0.2,0)*2*IF(IF(M60&gt;=384,0,M60)&gt;0,(384-M60)/384,0)*10000</f>
+        <f aca="false">MAX(N60-0.005,0)*MAX(ABS(L60)-0.25,0)*IF(IF(M60&gt;=384,0,M60)&gt;0,(384-M60)/384,0)*10000000</f>
         <v>0</v>
       </c>
     </row>
@@ -6480,7 +6497,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O61" s="17" t="e">
-        <f aca="false">MAX(N61-0.005,0)*100*MAX(ABS(L61)-0.2,0)*2*IF(IF(M61&gt;=384,0,M61)&gt;0,(384-M61)/384,0)*10000</f>
+        <f aca="false">MAX(N61-0.005,0)*MAX(ABS(L61)-0.25,0)*IF(IF(M61&gt;=384,0,M61)&gt;0,(384-M61)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6542,7 +6559,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O62" s="10" t="e">
-        <f aca="false">MAX(N62-0.005,0)*100*MAX(ABS(L62)-0.2,0)*2*IF(IF(M62&gt;=384,0,M62)&gt;0,(384-M62)/384,0)*10000</f>
+        <f aca="false">MAX(N62-0.005,0)*MAX(ABS(L62)-0.25,0)*IF(IF(M62&gt;=384,0,M62)&gt;0,(384-M62)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6604,7 +6621,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O63" s="17" t="e">
-        <f aca="false">MAX(N63-0.005,0)*100*MAX(ABS(L63)-0.2,0)*2*IF(IF(M63&gt;=384,0,M63)&gt;0,(384-M63)/384,0)*10000</f>
+        <f aca="false">MAX(N63-0.005,0)*MAX(ABS(L63)-0.25,0)*IF(IF(M63&gt;=384,0,M63)&gt;0,(384-M63)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6666,7 +6683,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O64" s="10" t="e">
-        <f aca="false">MAX(N64-0.005,0)*100*MAX(ABS(L64)-0.2,0)*2*IF(IF(M64&gt;=384,0,M64)&gt;0,(384-M64)/384,0)*10000</f>
+        <f aca="false">MAX(N64-0.005,0)*MAX(ABS(L64)-0.25,0)*IF(IF(M64&gt;=384,0,M64)&gt;0,(384-M64)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6728,7 +6745,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O65" s="17" t="e">
-        <f aca="false">MAX(N65-0.005,0)*100*MAX(ABS(L65)-0.2,0)*2*IF(IF(M65&gt;=384,0,M65)&gt;0,(384-M65)/384,0)*10000</f>
+        <f aca="false">MAX(N65-0.005,0)*MAX(ABS(L65)-0.25,0)*IF(IF(M65&gt;=384,0,M65)&gt;0,(384-M65)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6790,7 +6807,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O66" s="10" t="e">
-        <f aca="false">MAX(N66-0.005,0)*100*MAX(ABS(L66)-0.2,0)*2*IF(IF(M66&gt;=384,0,M66)&gt;0,(384-M66)/384,0)*10000</f>
+        <f aca="false">MAX(N66-0.005,0)*MAX(ABS(L66)-0.25,0)*IF(IF(M66&gt;=384,0,M66)&gt;0,(384-M66)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6852,7 +6869,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O67" s="17" t="e">
-        <f aca="false">MAX(N67-0.005,0)*100*MAX(ABS(L67)-0.2,0)*2*IF(IF(M67&gt;=384,0,M67)&gt;0,(384-M67)/384,0)*10000</f>
+        <f aca="false">MAX(N67-0.005,0)*MAX(ABS(L67)-0.25,0)*IF(IF(M67&gt;=384,0,M67)&gt;0,(384-M67)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6914,7 +6931,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O68" s="10" t="e">
-        <f aca="false">MAX(N68-0.005,0)*100*MAX(ABS(L68)-0.2,0)*2*IF(IF(M68&gt;=384,0,M68)&gt;0,(384-M68)/384,0)*10000</f>
+        <f aca="false">MAX(N68-0.005,0)*MAX(ABS(L68)-0.25,0)*IF(IF(M68&gt;=384,0,M68)&gt;0,(384-M68)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6976,7 +6993,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O69" s="17" t="e">
-        <f aca="false">MAX(N69-0.005,0)*100*MAX(ABS(L69)-0.2,0)*2*IF(IF(M69&gt;=384,0,M69)&gt;0,(384-M69)/384,0)*10000</f>
+        <f aca="false">MAX(N69-0.005,0)*MAX(ABS(L69)-0.25,0)*IF(IF(M69&gt;=384,0,M69)&gt;0,(384-M69)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7038,7 +7055,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O70" s="10" t="e">
-        <f aca="false">MAX(N70-0.005,0)*100*MAX(ABS(L70)-0.2,0)*2*IF(IF(M70&gt;=384,0,M70)&gt;0,(384-M70)/384,0)*10000</f>
+        <f aca="false">MAX(N70-0.005,0)*MAX(ABS(L70)-0.25,0)*IF(IF(M70&gt;=384,0,M70)&gt;0,(384-M70)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7100,7 +7117,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O71" s="17" t="e">
-        <f aca="false">MAX(N71-0.005,0)*100*MAX(ABS(L71)-0.2,0)*2*IF(IF(M71&gt;=384,0,M71)&gt;0,(384-M71)/384,0)*10000</f>
+        <f aca="false">MAX(N71-0.005,0)*MAX(ABS(L71)-0.25,0)*IF(IF(M71&gt;=384,0,M71)&gt;0,(384-M71)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7162,7 +7179,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O72" s="10" t="e">
-        <f aca="false">MAX(N72-0.005,0)*100*MAX(ABS(L72)-0.2,0)*2*IF(IF(M72&gt;=384,0,M72)&gt;0,(384-M72)/384,0)*10000</f>
+        <f aca="false">MAX(N72-0.005,0)*MAX(ABS(L72)-0.25,0)*IF(IF(M72&gt;=384,0,M72)&gt;0,(384-M72)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7224,7 +7241,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O73" s="17" t="e">
-        <f aca="false">MAX(N73-0.005,0)*100*MAX(ABS(L73)-0.2,0)*2*IF(IF(M73&gt;=384,0,M73)&gt;0,(384-M73)/384,0)*10000</f>
+        <f aca="false">MAX(N73-0.005,0)*MAX(ABS(L73)-0.25,0)*IF(IF(M73&gt;=384,0,M73)&gt;0,(384-M73)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7286,7 +7303,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O74" s="10" t="e">
-        <f aca="false">MAX(N74-0.005,0)*100*MAX(ABS(L74)-0.2,0)*2*IF(IF(M74&gt;=384,0,M74)&gt;0,(384-M74)/384,0)*10000</f>
+        <f aca="false">MAX(N74-0.005,0)*MAX(ABS(L74)-0.25,0)*IF(IF(M74&gt;=384,0,M74)&gt;0,(384-M74)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7348,7 +7365,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O75" s="17" t="e">
-        <f aca="false">MAX(N75-0.005,0)*100*MAX(ABS(L75)-0.2,0)*2*IF(IF(M75&gt;=384,0,M75)&gt;0,(384-M75)/384,0)*10000</f>
+        <f aca="false">MAX(N75-0.005,0)*MAX(ABS(L75)-0.25,0)*IF(IF(M75&gt;=384,0,M75)&gt;0,(384-M75)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7410,7 +7427,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O76" s="10" t="e">
-        <f aca="false">MAX(N76-0.005,0)*100*MAX(ABS(L76)-0.2,0)*2*IF(IF(M76&gt;=384,0,M76)&gt;0,(384-M76)/384,0)*10000</f>
+        <f aca="false">MAX(N76-0.005,0)*MAX(ABS(L76)-0.25,0)*IF(IF(M76&gt;=384,0,M76)&gt;0,(384-M76)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7472,7 +7489,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O77" s="17" t="e">
-        <f aca="false">MAX(N77-0.005,0)*100*MAX(ABS(L77)-0.2,0)*2*IF(IF(M77&gt;=384,0,M77)&gt;0,(384-M77)/384,0)*10000</f>
+        <f aca="false">MAX(N77-0.005,0)*MAX(ABS(L77)-0.25,0)*IF(IF(M77&gt;=384,0,M77)&gt;0,(384-M77)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7534,7 +7551,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O78" s="10" t="e">
-        <f aca="false">MAX(N78-0.005,0)*100*MAX(ABS(L78)-0.2,0)*2*IF(IF(M78&gt;=384,0,M78)&gt;0,(384-M78)/384,0)*10000</f>
+        <f aca="false">MAX(N78-0.005,0)*MAX(ABS(L78)-0.25,0)*IF(IF(M78&gt;=384,0,M78)&gt;0,(384-M78)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7596,7 +7613,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O79" s="17" t="e">
-        <f aca="false">MAX(N79-0.005,0)*100*MAX(ABS(L79)-0.2,0)*2*IF(IF(M79&gt;=384,0,M79)&gt;0,(384-M79)/384,0)*10000</f>
+        <f aca="false">MAX(N79-0.005,0)*MAX(ABS(L79)-0.25,0)*IF(IF(M79&gt;=384,0,M79)&gt;0,(384-M79)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7658,7 +7675,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O80" s="10" t="e">
-        <f aca="false">MAX(N80-0.005,0)*100*MAX(ABS(L80)-0.2,0)*2*IF(IF(M80&gt;=384,0,M80)&gt;0,(384-M80)/384,0)*10000</f>
+        <f aca="false">MAX(N80-0.005,0)*MAX(ABS(L80)-0.25,0)*IF(IF(M80&gt;=384,0,M80)&gt;0,(384-M80)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7720,7 +7737,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O81" s="17" t="e">
-        <f aca="false">MAX(N81-0.005,0)*100*MAX(ABS(L81)-0.2,0)*2*IF(IF(M81&gt;=384,0,M81)&gt;0,(384-M81)/384,0)*10000</f>
+        <f aca="false">MAX(N81-0.005,0)*MAX(ABS(L81)-0.25,0)*IF(IF(M81&gt;=384,0,M81)&gt;0,(384-M81)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7782,7 +7799,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O82" s="10" t="e">
-        <f aca="false">MAX(N82-0.005,0)*100*MAX(ABS(L82)-0.2,0)*2*IF(IF(M82&gt;=384,0,M82)&gt;0,(384-M82)/384,0)*10000</f>
+        <f aca="false">MAX(N82-0.005,0)*MAX(ABS(L82)-0.25,0)*IF(IF(M82&gt;=384,0,M82)&gt;0,(384-M82)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7844,7 +7861,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O83" s="17" t="e">
-        <f aca="false">MAX(N83-0.005,0)*100*MAX(ABS(L83)-0.2,0)*2*IF(IF(M83&gt;=384,0,M83)&gt;0,(384-M83)/384,0)*10000</f>
+        <f aca="false">MAX(N83-0.005,0)*MAX(ABS(L83)-0.25,0)*IF(IF(M83&gt;=384,0,M83)&gt;0,(384-M83)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7906,7 +7923,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O84" s="10" t="e">
-        <f aca="false">MAX(N84-0.005,0)*100*MAX(ABS(L84)-0.2,0)*2*IF(IF(M84&gt;=384,0,M84)&gt;0,(384-M84)/384,0)*10000</f>
+        <f aca="false">MAX(N84-0.005,0)*MAX(ABS(L84)-0.25,0)*IF(IF(M84&gt;=384,0,M84)&gt;0,(384-M84)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7968,7 +7985,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O85" s="17" t="e">
-        <f aca="false">MAX(N85-0.005,0)*100*MAX(ABS(L85)-0.2,0)*2*IF(IF(M85&gt;=384,0,M85)&gt;0,(384-M85)/384,0)*10000</f>
+        <f aca="false">MAX(N85-0.005,0)*MAX(ABS(L85)-0.25,0)*IF(IF(M85&gt;=384,0,M85)&gt;0,(384-M85)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8030,7 +8047,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O86" s="10" t="e">
-        <f aca="false">MAX(N86-0.005,0)*100*MAX(ABS(L86)-0.2,0)*2*IF(IF(M86&gt;=384,0,M86)&gt;0,(384-M86)/384,0)*10000</f>
+        <f aca="false">MAX(N86-0.005,0)*MAX(ABS(L86)-0.25,0)*IF(IF(M86&gt;=384,0,M86)&gt;0,(384-M86)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8092,7 +8109,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O87" s="17" t="e">
-        <f aca="false">MAX(N87-0.005,0)*100*MAX(ABS(L87)-0.2,0)*2*IF(IF(M87&gt;=384,0,M87)&gt;0,(384-M87)/384,0)*10000</f>
+        <f aca="false">MAX(N87-0.005,0)*MAX(ABS(L87)-0.25,0)*IF(IF(M87&gt;=384,0,M87)&gt;0,(384-M87)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8154,7 +8171,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O88" s="10" t="e">
-        <f aca="false">MAX(N88-0.005,0)*100*MAX(ABS(L88)-0.2,0)*2*IF(IF(M88&gt;=384,0,M88)&gt;0,(384-M88)/384,0)*10000</f>
+        <f aca="false">MAX(N88-0.005,0)*MAX(ABS(L88)-0.25,0)*IF(IF(M88&gt;=384,0,M88)&gt;0,(384-M88)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8216,7 +8233,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O89" s="17" t="e">
-        <f aca="false">MAX(N89-0.005,0)*100*MAX(ABS(L89)-0.2,0)*2*IF(IF(M89&gt;=384,0,M89)&gt;0,(384-M89)/384,0)*10000</f>
+        <f aca="false">MAX(N89-0.005,0)*MAX(ABS(L89)-0.25,0)*IF(IF(M89&gt;=384,0,M89)&gt;0,(384-M89)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8278,7 +8295,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O90" s="10" t="e">
-        <f aca="false">MAX(N90-0.005,0)*100*MAX(ABS(L90)-0.2,0)*2*IF(IF(M90&gt;=384,0,M90)&gt;0,(384-M90)/384,0)*10000</f>
+        <f aca="false">MAX(N90-0.005,0)*MAX(ABS(L90)-0.25,0)*IF(IF(M90&gt;=384,0,M90)&gt;0,(384-M90)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8340,7 +8357,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O91" s="17" t="e">
-        <f aca="false">MAX(N91-0.005,0)*100*MAX(ABS(L91)-0.2,0)*2*IF(IF(M91&gt;=384,0,M91)&gt;0,(384-M91)/384,0)*10000</f>
+        <f aca="false">MAX(N91-0.005,0)*MAX(ABS(L91)-0.25,0)*IF(IF(M91&gt;=384,0,M91)&gt;0,(384-M91)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8402,7 +8419,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O92" s="10" t="e">
-        <f aca="false">MAX(N92-0.005,0)*100*MAX(ABS(L92)-0.2,0)*2*IF(IF(M92&gt;=384,0,M92)&gt;0,(384-M92)/384,0)*10000</f>
+        <f aca="false">MAX(N92-0.005,0)*MAX(ABS(L92)-0.25,0)*IF(IF(M92&gt;=384,0,M92)&gt;0,(384-M92)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8464,7 +8481,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O93" s="17" t="e">
-        <f aca="false">MAX(N93-0.005,0)*100*MAX(ABS(L93)-0.2,0)*2*IF(IF(M93&gt;=384,0,M93)&gt;0,(384-M93)/384,0)*10000</f>
+        <f aca="false">MAX(N93-0.005,0)*MAX(ABS(L93)-0.25,0)*IF(IF(M93&gt;=384,0,M93)&gt;0,(384-M93)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8526,7 +8543,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O94" s="10" t="e">
-        <f aca="false">MAX(N94-0.005,0)*100*MAX(ABS(L94)-0.2,0)*2*IF(IF(M94&gt;=384,0,M94)&gt;0,(384-M94)/384,0)*10000</f>
+        <f aca="false">MAX(N94-0.005,0)*MAX(ABS(L94)-0.25,0)*IF(IF(M94&gt;=384,0,M94)&gt;0,(384-M94)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8588,7 +8605,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O95" s="17" t="e">
-        <f aca="false">MAX(N95-0.005,0)*100*MAX(ABS(L95)-0.2,0)*2*IF(IF(M95&gt;=384,0,M95)&gt;0,(384-M95)/384,0)*10000</f>
+        <f aca="false">MAX(N95-0.005,0)*MAX(ABS(L95)-0.25,0)*IF(IF(M95&gt;=384,0,M95)&gt;0,(384-M95)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8650,7 +8667,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O96" s="10" t="e">
-        <f aca="false">MAX(N96-0.005,0)*100*MAX(ABS(L96)-0.2,0)*2*IF(IF(M96&gt;=384,0,M96)&gt;0,(384-M96)/384,0)*10000</f>
+        <f aca="false">MAX(N96-0.005,0)*MAX(ABS(L96)-0.25,0)*IF(IF(M96&gt;=384,0,M96)&gt;0,(384-M96)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8712,7 +8729,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O97" s="17" t="e">
-        <f aca="false">MAX(N97-0.005,0)*100*MAX(ABS(L97)-0.2,0)*2*IF(IF(M97&gt;=384,0,M97)&gt;0,(384-M97)/384,0)*10000</f>
+        <f aca="false">MAX(N97-0.005,0)*MAX(ABS(L97)-0.25,0)*IF(IF(M97&gt;=384,0,M97)&gt;0,(384-M97)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8774,7 +8791,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O98" s="10" t="e">
-        <f aca="false">MAX(N98-0.005,0)*100*MAX(ABS(L98)-0.2,0)*2*IF(IF(M98&gt;=384,0,M98)&gt;0,(384-M98)/384,0)*10000</f>
+        <f aca="false">MAX(N98-0.005,0)*MAX(ABS(L98)-0.25,0)*IF(IF(M98&gt;=384,0,M98)&gt;0,(384-M98)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8836,7 +8853,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O99" s="17" t="e">
-        <f aca="false">MAX(N99-0.005,0)*100*MAX(ABS(L99)-0.2,0)*2*IF(IF(M99&gt;=384,0,M99)&gt;0,(384-M99)/384,0)*10000</f>
+        <f aca="false">MAX(N99-0.005,0)*MAX(ABS(L99)-0.25,0)*IF(IF(M99&gt;=384,0,M99)&gt;0,(384-M99)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8898,7 +8915,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O100" s="10" t="e">
-        <f aca="false">MAX(N100-0.005,0)*100*MAX(ABS(L100)-0.2,0)*2*IF(IF(M100&gt;=384,0,M100)&gt;0,(384-M100)/384,0)*10000</f>
+        <f aca="false">MAX(N100-0.005,0)*MAX(ABS(L100)-0.25,0)*IF(IF(M100&gt;=384,0,M100)&gt;0,(384-M100)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8960,7 +8977,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O101" s="17" t="e">
-        <f aca="false">MAX(N101-0.005,0)*100*MAX(ABS(L101)-0.2,0)*2*IF(IF(M101&gt;=384,0,M101)&gt;0,(384-M101)/384,0)*10000</f>
+        <f aca="false">MAX(N101-0.005,0)*MAX(ABS(L101)-0.25,0)*IF(IF(M101&gt;=384,0,M101)&gt;0,(384-M101)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9022,7 +9039,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O102" s="10" t="e">
-        <f aca="false">MAX(N102-0.005,0)*100*MAX(ABS(L102)-0.2,0)*2*IF(IF(M102&gt;=384,0,M102)&gt;0,(384-M102)/384,0)*10000</f>
+        <f aca="false">MAX(N102-0.005,0)*MAX(ABS(L102)-0.25,0)*IF(IF(M102&gt;=384,0,M102)&gt;0,(384-M102)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9084,7 +9101,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O103" s="17" t="e">
-        <f aca="false">MAX(N103-0.005,0)*100*MAX(ABS(L103)-0.2,0)*2*IF(IF(M103&gt;=384,0,M103)&gt;0,(384-M103)/384,0)*10000</f>
+        <f aca="false">MAX(N103-0.005,0)*MAX(ABS(L103)-0.25,0)*IF(IF(M103&gt;=384,0,M103)&gt;0,(384-M103)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9146,7 +9163,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O104" s="10" t="e">
-        <f aca="false">MAX(N104-0.005,0)*100*MAX(ABS(L104)-0.2,0)*2*IF(IF(M104&gt;=384,0,M104)&gt;0,(384-M104)/384,0)*10000</f>
+        <f aca="false">MAX(N104-0.005,0)*MAX(ABS(L104)-0.25,0)*IF(IF(M104&gt;=384,0,M104)&gt;0,(384-M104)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9208,7 +9225,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O105" s="17" t="e">
-        <f aca="false">MAX(N105-0.005,0)*100*MAX(ABS(L105)-0.2,0)*2*IF(IF(M105&gt;=384,0,M105)&gt;0,(384-M105)/384,0)*10000</f>
+        <f aca="false">MAX(N105-0.005,0)*MAX(ABS(L105)-0.25,0)*IF(IF(M105&gt;=384,0,M105)&gt;0,(384-M105)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9270,7 +9287,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O106" s="10" t="e">
-        <f aca="false">MAX(N106-0.005,0)*100*MAX(ABS(L106)-0.2,0)*2*IF(IF(M106&gt;=384,0,M106)&gt;0,(384-M106)/384,0)*10000</f>
+        <f aca="false">MAX(N106-0.005,0)*MAX(ABS(L106)-0.25,0)*IF(IF(M106&gt;=384,0,M106)&gt;0,(384-M106)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9332,7 +9349,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O107" s="17" t="e">
-        <f aca="false">MAX(N107-0.005,0)*100*MAX(ABS(L107)-0.2,0)*2*IF(IF(M107&gt;=384,0,M107)&gt;0,(384-M107)/384,0)*10000</f>
+        <f aca="false">MAX(N107-0.005,0)*MAX(ABS(L107)-0.25,0)*IF(IF(M107&gt;=384,0,M107)&gt;0,(384-M107)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9394,7 +9411,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O108" s="10" t="e">
-        <f aca="false">MAX(N108-0.005,0)*100*MAX(ABS(L108)-0.2,0)*2*IF(IF(M108&gt;=384,0,M108)&gt;0,(384-M108)/384,0)*10000</f>
+        <f aca="false">MAX(N108-0.005,0)*MAX(ABS(L108)-0.25,0)*IF(IF(M108&gt;=384,0,M108)&gt;0,(384-M108)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9456,7 +9473,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O109" s="17" t="e">
-        <f aca="false">MAX(N109-0.005,0)*100*MAX(ABS(L109)-0.2,0)*2*IF(IF(M109&gt;=384,0,M109)&gt;0,(384-M109)/384,0)*10000</f>
+        <f aca="false">MAX(N109-0.005,0)*MAX(ABS(L109)-0.25,0)*IF(IF(M109&gt;=384,0,M109)&gt;0,(384-M109)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9518,7 +9535,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O110" s="10" t="e">
-        <f aca="false">MAX(N110-0.005,0)*100*MAX(ABS(L110)-0.2,0)*2*IF(IF(M110&gt;=384,0,M110)&gt;0,(384-M110)/384,0)*10000</f>
+        <f aca="false">MAX(N110-0.005,0)*MAX(ABS(L110)-0.25,0)*IF(IF(M110&gt;=384,0,M110)&gt;0,(384-M110)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9580,7 +9597,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O111" s="17" t="e">
-        <f aca="false">MAX(N111-0.005,0)*100*MAX(ABS(L111)-0.2,0)*2*IF(IF(M111&gt;=384,0,M111)&gt;0,(384-M111)/384,0)*10000</f>
+        <f aca="false">MAX(N111-0.005,0)*MAX(ABS(L111)-0.25,0)*IF(IF(M111&gt;=384,0,M111)&gt;0,(384-M111)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9642,7 +9659,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O112" s="10" t="e">
-        <f aca="false">MAX(N112-0.005,0)*100*MAX(ABS(L112)-0.2,0)*2*IF(IF(M112&gt;=384,0,M112)&gt;0,(384-M112)/384,0)*10000</f>
+        <f aca="false">MAX(N112-0.005,0)*MAX(ABS(L112)-0.25,0)*IF(IF(M112&gt;=384,0,M112)&gt;0,(384-M112)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9704,7 +9721,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O113" s="17" t="e">
-        <f aca="false">MAX(N113-0.005,0)*100*MAX(ABS(L113)-0.2,0)*2*IF(IF(M113&gt;=384,0,M113)&gt;0,(384-M113)/384,0)*10000</f>
+        <f aca="false">MAX(N113-0.005,0)*MAX(ABS(L113)-0.25,0)*IF(IF(M113&gt;=384,0,M113)&gt;0,(384-M113)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9766,7 +9783,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O114" s="10" t="e">
-        <f aca="false">MAX(N114-0.005,0)*100*MAX(ABS(L114)-0.2,0)*2*IF(IF(M114&gt;=384,0,M114)&gt;0,(384-M114)/384,0)*10000</f>
+        <f aca="false">MAX(N114-0.005,0)*MAX(ABS(L114)-0.25,0)*IF(IF(M114&gt;=384,0,M114)&gt;0,(384-M114)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9828,7 +9845,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O115" s="17" t="e">
-        <f aca="false">MAX(N115-0.005,0)*100*MAX(ABS(L115)-0.2,0)*2*IF(IF(M115&gt;=384,0,M115)&gt;0,(384-M115)/384,0)*10000</f>
+        <f aca="false">MAX(N115-0.005,0)*MAX(ABS(L115)-0.25,0)*IF(IF(M115&gt;=384,0,M115)&gt;0,(384-M115)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9890,7 +9907,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O116" s="10" t="e">
-        <f aca="false">MAX(N116-0.005,0)*100*MAX(ABS(L116)-0.2,0)*2*IF(IF(M116&gt;=384,0,M116)&gt;0,(384-M116)/384,0)*10000</f>
+        <f aca="false">MAX(N116-0.005,0)*MAX(ABS(L116)-0.25,0)*IF(IF(M116&gt;=384,0,M116)&gt;0,(384-M116)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9952,7 +9969,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O117" s="17" t="e">
-        <f aca="false">MAX(N117-0.005,0)*100*MAX(ABS(L117)-0.2,0)*2*IF(IF(M117&gt;=384,0,M117)&gt;0,(384-M117)/384,0)*10000</f>
+        <f aca="false">MAX(N117-0.005,0)*MAX(ABS(L117)-0.25,0)*IF(IF(M117&gt;=384,0,M117)&gt;0,(384-M117)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10014,7 +10031,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O118" s="10" t="e">
-        <f aca="false">MAX(N118-0.005,0)*100*MAX(ABS(L118)-0.2,0)*2*IF(IF(M118&gt;=384,0,M118)&gt;0,(384-M118)/384,0)*10000</f>
+        <f aca="false">MAX(N118-0.005,0)*MAX(ABS(L118)-0.25,0)*IF(IF(M118&gt;=384,0,M118)&gt;0,(384-M118)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10076,7 +10093,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O119" s="17" t="e">
-        <f aca="false">MAX(N119-0.005,0)*100*MAX(ABS(L119)-0.2,0)*2*IF(IF(M119&gt;=384,0,M119)&gt;0,(384-M119)/384,0)*10000</f>
+        <f aca="false">MAX(N119-0.005,0)*MAX(ABS(L119)-0.25,0)*IF(IF(M119&gt;=384,0,M119)&gt;0,(384-M119)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10138,7 +10155,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O120" s="10" t="e">
-        <f aca="false">MAX(N120-0.005,0)*100*MAX(ABS(L120)-0.2,0)*2*IF(IF(M120&gt;=384,0,M120)&gt;0,(384-M120)/384,0)*10000</f>
+        <f aca="false">MAX(N120-0.005,0)*MAX(ABS(L120)-0.25,0)*IF(IF(M120&gt;=384,0,M120)&gt;0,(384-M120)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10200,7 +10217,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O121" s="17" t="e">
-        <f aca="false">MAX(N121-0.005,0)*100*MAX(ABS(L121)-0.2,0)*2*IF(IF(M121&gt;=384,0,M121)&gt;0,(384-M121)/384,0)*10000</f>
+        <f aca="false">MAX(N121-0.005,0)*MAX(ABS(L121)-0.25,0)*IF(IF(M121&gt;=384,0,M121)&gt;0,(384-M121)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10262,7 +10279,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O122" s="10" t="e">
-        <f aca="false">MAX(N122-0.005,0)*100*MAX(ABS(L122)-0.2,0)*2*IF(IF(M122&gt;=384,0,M122)&gt;0,(384-M122)/384,0)*10000</f>
+        <f aca="false">MAX(N122-0.005,0)*MAX(ABS(L122)-0.25,0)*IF(IF(M122&gt;=384,0,M122)&gt;0,(384-M122)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10324,7 +10341,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O123" s="17" t="e">
-        <f aca="false">MAX(N123-0.005,0)*100*MAX(ABS(L123)-0.2,0)*2*IF(IF(M123&gt;=384,0,M123)&gt;0,(384-M123)/384,0)*10000</f>
+        <f aca="false">MAX(N123-0.005,0)*MAX(ABS(L123)-0.25,0)*IF(IF(M123&gt;=384,0,M123)&gt;0,(384-M123)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10386,7 +10403,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O124" s="10" t="e">
-        <f aca="false">MAX(N124-0.005,0)*100*MAX(ABS(L124)-0.2,0)*2*IF(IF(M124&gt;=384,0,M124)&gt;0,(384-M124)/384,0)*10000</f>
+        <f aca="false">MAX(N124-0.005,0)*MAX(ABS(L124)-0.25,0)*IF(IF(M124&gt;=384,0,M124)&gt;0,(384-M124)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10448,7 +10465,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O125" s="17" t="e">
-        <f aca="false">MAX(N125-0.005,0)*100*MAX(ABS(L125)-0.2,0)*2*IF(IF(M125&gt;=384,0,M125)&gt;0,(384-M125)/384,0)*10000</f>
+        <f aca="false">MAX(N125-0.005,0)*MAX(ABS(L125)-0.25,0)*IF(IF(M125&gt;=384,0,M125)&gt;0,(384-M125)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10510,7 +10527,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O126" s="10" t="e">
-        <f aca="false">MAX(N126-0.005,0)*100*MAX(ABS(L126)-0.2,0)*2*IF(IF(M126&gt;=384,0,M126)&gt;0,(384-M126)/384,0)*10000</f>
+        <f aca="false">MAX(N126-0.005,0)*MAX(ABS(L126)-0.25,0)*IF(IF(M126&gt;=384,0,M126)&gt;0,(384-M126)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10572,7 +10589,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O127" s="17" t="e">
-        <f aca="false">MAX(N127-0.005,0)*100*MAX(ABS(L127)-0.2,0)*2*IF(IF(M127&gt;=384,0,M127)&gt;0,(384-M127)/384,0)*10000</f>
+        <f aca="false">MAX(N127-0.005,0)*MAX(ABS(L127)-0.25,0)*IF(IF(M127&gt;=384,0,M127)&gt;0,(384-M127)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10634,7 +10651,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O128" s="10" t="e">
-        <f aca="false">MAX(N128-0.005,0)*100*MAX(ABS(L128)-0.2,0)*2*IF(IF(M128&gt;=384,0,M128)&gt;0,(384-M128)/384,0)*10000</f>
+        <f aca="false">MAX(N128-0.005,0)*MAX(ABS(L128)-0.25,0)*IF(IF(M128&gt;=384,0,M128)&gt;0,(384-M128)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10696,7 +10713,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O129" s="17" t="e">
-        <f aca="false">MAX(N129-0.005,0)*100*MAX(ABS(L129)-0.2,0)*2*IF(IF(M129&gt;=384,0,M129)&gt;0,(384-M129)/384,0)*10000</f>
+        <f aca="false">MAX(N129-0.005,0)*MAX(ABS(L129)-0.25,0)*IF(IF(M129&gt;=384,0,M129)&gt;0,(384-M129)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10758,7 +10775,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O130" s="10" t="e">
-        <f aca="false">MAX(N130-0.005,0)*100*MAX(ABS(L130)-0.2,0)*2*IF(IF(M130&gt;=384,0,M130)&gt;0,(384-M130)/384,0)*10000</f>
+        <f aca="false">MAX(N130-0.005,0)*MAX(ABS(L130)-0.25,0)*IF(IF(M130&gt;=384,0,M130)&gt;0,(384-M130)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10820,7 +10837,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O131" s="17" t="e">
-        <f aca="false">MAX(N131-0.005,0)*100*MAX(ABS(L131)-0.2,0)*2*IF(IF(M131&gt;=384,0,M131)&gt;0,(384-M131)/384,0)*10000</f>
+        <f aca="false">MAX(N131-0.005,0)*MAX(ABS(L131)-0.25,0)*IF(IF(M131&gt;=384,0,M131)&gt;0,(384-M131)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10882,7 +10899,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O132" s="10" t="e">
-        <f aca="false">MAX(N132-0.005,0)*100*MAX(ABS(L132)-0.2,0)*2*IF(IF(M132&gt;=384,0,M132)&gt;0,(384-M132)/384,0)*10000</f>
+        <f aca="false">MAX(N132-0.005,0)*MAX(ABS(L132)-0.25,0)*IF(IF(M132&gt;=384,0,M132)&gt;0,(384-M132)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10944,7 +10961,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O133" s="17" t="e">
-        <f aca="false">MAX(N133-0.005,0)*100*MAX(ABS(L133)-0.2,0)*2*IF(IF(M133&gt;=384,0,M133)&gt;0,(384-M133)/384,0)*10000</f>
+        <f aca="false">MAX(N133-0.005,0)*MAX(ABS(L133)-0.25,0)*IF(IF(M133&gt;=384,0,M133)&gt;0,(384-M133)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11006,7 +11023,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O134" s="10" t="e">
-        <f aca="false">MAX(N134-0.005,0)*100*MAX(ABS(L134)-0.2,0)*2*IF(IF(M134&gt;=384,0,M134)&gt;0,(384-M134)/384,0)*10000</f>
+        <f aca="false">MAX(N134-0.005,0)*MAX(ABS(L134)-0.25,0)*IF(IF(M134&gt;=384,0,M134)&gt;0,(384-M134)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11068,7 +11085,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O135" s="17" t="e">
-        <f aca="false">MAX(N135-0.005,0)*100*MAX(ABS(L135)-0.2,0)*2*IF(IF(M135&gt;=384,0,M135)&gt;0,(384-M135)/384,0)*10000</f>
+        <f aca="false">MAX(N135-0.005,0)*MAX(ABS(L135)-0.25,0)*IF(IF(M135&gt;=384,0,M135)&gt;0,(384-M135)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11130,7 +11147,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O136" s="10" t="e">
-        <f aca="false">MAX(N136-0.005,0)*100*MAX(ABS(L136)-0.2,0)*2*IF(IF(M136&gt;=384,0,M136)&gt;0,(384-M136)/384,0)*10000</f>
+        <f aca="false">MAX(N136-0.005,0)*MAX(ABS(L136)-0.25,0)*IF(IF(M136&gt;=384,0,M136)&gt;0,(384-M136)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11192,7 +11209,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O137" s="17" t="e">
-        <f aca="false">MAX(N137-0.005,0)*100*MAX(ABS(L137)-0.2,0)*2*IF(IF(M137&gt;=384,0,M137)&gt;0,(384-M137)/384,0)*10000</f>
+        <f aca="false">MAX(N137-0.005,0)*MAX(ABS(L137)-0.25,0)*IF(IF(M137&gt;=384,0,M137)&gt;0,(384-M137)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11254,7 +11271,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O138" s="10" t="e">
-        <f aca="false">MAX(N138-0.005,0)*100*MAX(ABS(L138)-0.2,0)*2*IF(IF(M138&gt;=384,0,M138)&gt;0,(384-M138)/384,0)*10000</f>
+        <f aca="false">MAX(N138-0.005,0)*MAX(ABS(L138)-0.25,0)*IF(IF(M138&gt;=384,0,M138)&gt;0,(384-M138)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11316,7 +11333,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O139" s="17" t="e">
-        <f aca="false">MAX(N139-0.005,0)*100*MAX(ABS(L139)-0.2,0)*2*IF(IF(M139&gt;=384,0,M139)&gt;0,(384-M139)/384,0)*10000</f>
+        <f aca="false">MAX(N139-0.005,0)*MAX(ABS(L139)-0.25,0)*IF(IF(M139&gt;=384,0,M139)&gt;0,(384-M139)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11378,7 +11395,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O140" s="10" t="e">
-        <f aca="false">MAX(N140-0.005,0)*100*MAX(ABS(L140)-0.2,0)*2*IF(IF(M140&gt;=384,0,M140)&gt;0,(384-M140)/384,0)*10000</f>
+        <f aca="false">MAX(N140-0.005,0)*MAX(ABS(L140)-0.25,0)*IF(IF(M140&gt;=384,0,M140)&gt;0,(384-M140)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11440,7 +11457,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O141" s="17" t="e">
-        <f aca="false">MAX(N141-0.005,0)*100*MAX(ABS(L141)-0.2,0)*2*IF(IF(M141&gt;=384,0,M141)&gt;0,(384-M141)/384,0)*10000</f>
+        <f aca="false">MAX(N141-0.005,0)*MAX(ABS(L141)-0.25,0)*IF(IF(M141&gt;=384,0,M141)&gt;0,(384-M141)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11502,7 +11519,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O142" s="10" t="e">
-        <f aca="false">MAX(N142-0.005,0)*100*MAX(ABS(L142)-0.2,0)*2*IF(IF(M142&gt;=384,0,M142)&gt;0,(384-M142)/384,0)*10000</f>
+        <f aca="false">MAX(N142-0.005,0)*MAX(ABS(L142)-0.25,0)*IF(IF(M142&gt;=384,0,M142)&gt;0,(384-M142)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11564,7 +11581,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O143" s="17" t="e">
-        <f aca="false">MAX(N143-0.005,0)*100*MAX(ABS(L143)-0.2,0)*2*IF(IF(M143&gt;=384,0,M143)&gt;0,(384-M143)/384,0)*10000</f>
+        <f aca="false">MAX(N143-0.005,0)*MAX(ABS(L143)-0.25,0)*IF(IF(M143&gt;=384,0,M143)&gt;0,(384-M143)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11626,7 +11643,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O144" s="10" t="e">
-        <f aca="false">MAX(N144-0.005,0)*100*MAX(ABS(L144)-0.2,0)*2*IF(IF(M144&gt;=384,0,M144)&gt;0,(384-M144)/384,0)*10000</f>
+        <f aca="false">MAX(N144-0.005,0)*MAX(ABS(L144)-0.25,0)*IF(IF(M144&gt;=384,0,M144)&gt;0,(384-M144)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11688,7 +11705,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O145" s="17" t="e">
-        <f aca="false">MAX(N145-0.005,0)*100*MAX(ABS(L145)-0.2,0)*2*IF(IF(M145&gt;=384,0,M145)&gt;0,(384-M145)/384,0)*10000</f>
+        <f aca="false">MAX(N145-0.005,0)*MAX(ABS(L145)-0.25,0)*IF(IF(M145&gt;=384,0,M145)&gt;0,(384-M145)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11750,7 +11767,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O146" s="10" t="e">
-        <f aca="false">MAX(N146-0.005,0)*100*MAX(ABS(L146)-0.2,0)*2*IF(IF(M146&gt;=384,0,M146)&gt;0,(384-M146)/384,0)*10000</f>
+        <f aca="false">MAX(N146-0.005,0)*MAX(ABS(L146)-0.25,0)*IF(IF(M146&gt;=384,0,M146)&gt;0,(384-M146)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11812,7 +11829,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O147" s="17" t="e">
-        <f aca="false">MAX(N147-0.005,0)*100*MAX(ABS(L147)-0.2,0)*2*IF(IF(M147&gt;=384,0,M147)&gt;0,(384-M147)/384,0)*10000</f>
+        <f aca="false">MAX(N147-0.005,0)*MAX(ABS(L147)-0.25,0)*IF(IF(M147&gt;=384,0,M147)&gt;0,(384-M147)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11874,7 +11891,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O148" s="10" t="e">
-        <f aca="false">MAX(N148-0.005,0)*100*MAX(ABS(L148)-0.2,0)*2*IF(IF(M148&gt;=384,0,M148)&gt;0,(384-M148)/384,0)*10000</f>
+        <f aca="false">MAX(N148-0.005,0)*MAX(ABS(L148)-0.25,0)*IF(IF(M148&gt;=384,0,M148)&gt;0,(384-M148)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11936,7 +11953,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O149" s="17" t="e">
-        <f aca="false">MAX(N149-0.005,0)*100*MAX(ABS(L149)-0.2,0)*2*IF(IF(M149&gt;=384,0,M149)&gt;0,(384-M149)/384,0)*10000</f>
+        <f aca="false">MAX(N149-0.005,0)*MAX(ABS(L149)-0.25,0)*IF(IF(M149&gt;=384,0,M149)&gt;0,(384-M149)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -11998,13 +12015,13 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O150" s="10" t="e">
-        <f aca="false">MAX(N150-0.005,0)*100*MAX(ABS(L150)-0.2,0)*2*IF(IF(M150&gt;=384,0,M150)&gt;0,(384-M150)/384,0)*10000</f>
+        <f aca="false">MAX(N150-0.005,0)*MAX(ABS(L150)-0.25,0)*IF(IF(M150&gt;=384,0,M150)&gt;0,(384-M150)/384,0)*10000000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:O100"/>
-  <conditionalFormatting sqref="A1:O150">
+  <conditionalFormatting sqref="A1:O2 A3:N150 O3:O151">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>MOD(ROW()),2)=0</formula>
     </cfRule>

</xml_diff>